<commit_message>
commit on 14 april
</commit_message>
<xml_diff>
--- a/public/general_file/Add_Lead.xlsx
+++ b/public/general_file/Add_Lead.xlsx
@@ -1,51 +1,84 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="630" windowWidth="19815" windowHeight="6600"/>
+  </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Product Qty</t>
+  </si>
+  <si>
+    <t>Product Amount</t>
+  </si>
+  <si>
+    <t>Product SubTotal Amount</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>Lead Stage</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Another Phone Number</t>
+  </si>
+  <si>
+    <t>Owner Name</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <b/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -54,20 +87,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -392,56 +428,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.8515625" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.00390625" customWidth="1"/>
-    <col min="5" max="5" width="8.421875" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.57421875" customWidth="1"/>
-    <col min="8" max="8" width="14.57421875" customWidth="1"/>
-    <col min="9" max="9" width="8.28125" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="14.75" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="15.375" customWidth="1"/>
+    <col min="10" max="10" width="27.625" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>First Name</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Last Name</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Company Name</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <v>Email</v>
-      </c>
-      <c r="E1" s="3" t="str">
-        <v>Product Name</v>
-      </c>
-      <c r="F1" s="3" t="str">
-        <v>Product Qty</v>
-      </c>
-      <c r="G1" s="3" t="str">
-        <v>Product Amount</v>
-      </c>
-      <c r="H1" s="3" t="str">
-        <v>Product SubTotal Amount</v>
-      </c>
-      <c r="I1" s="3" t="str">
-        <v>Total Amount</v>
-      </c>
-      <c r="J1" s="3" t="str">
-        <v>Lead Stage</v>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>